<commit_message>
Remove international bunker fuels and align domestic shipping emissions with inventory
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\trans\AVLo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BE0324-6536-42D8-B7FD-1FCDBFD8F9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BA3925-3EC3-4BAA-8E29-F5A0D5FA67BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9980" yWindow="550" windowWidth="15430" windowHeight="12970" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -24,11 +24,12 @@
     <sheet name="고속철도 여객수송동향" sheetId="14" r:id="rId9"/>
     <sheet name="열차 여객수송인원" sheetId="15" r:id="rId10"/>
     <sheet name="rail" sheetId="13" r:id="rId11"/>
-    <sheet name="AVLo-passengers" sheetId="2" r:id="rId12"/>
-    <sheet name="AVLo-freight" sheetId="4" r:id="rId13"/>
+    <sheet name="US AVLo" sheetId="17" r:id="rId12"/>
+    <sheet name="AVLo-passengers" sheetId="2" r:id="rId13"/>
+    <sheet name="AVLo-freight" sheetId="4" r:id="rId14"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="Eno_TM">'[1]1997  Table 1a Modified'!#REF!</definedName>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="497">
   <si>
     <t>AVLo Average Vehicle Loading</t>
   </si>
@@ -3256,7 +3257,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3608,6 +3609,7 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="155">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4462,7 +4464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -6080,6 +6082,1582 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8AABE4-9A7A-4FF9-8C38-25844DE09CA8}">
+  <dimension ref="A1:AK15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:37">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>2015</v>
+      </c>
+      <c r="C1">
+        <v>2016</v>
+      </c>
+      <c r="D1">
+        <v>2017</v>
+      </c>
+      <c r="E1">
+        <v>2018</v>
+      </c>
+      <c r="F1">
+        <v>2019</v>
+      </c>
+      <c r="G1">
+        <v>2020</v>
+      </c>
+      <c r="H1">
+        <v>2021</v>
+      </c>
+      <c r="I1">
+        <v>2022</v>
+      </c>
+      <c r="J1">
+        <v>2023</v>
+      </c>
+      <c r="K1">
+        <v>2024</v>
+      </c>
+      <c r="L1">
+        <v>2025</v>
+      </c>
+      <c r="M1">
+        <v>2026</v>
+      </c>
+      <c r="N1">
+        <v>2027</v>
+      </c>
+      <c r="O1">
+        <v>2028</v>
+      </c>
+      <c r="P1">
+        <v>2029</v>
+      </c>
+      <c r="Q1">
+        <v>2030</v>
+      </c>
+      <c r="R1">
+        <v>2031</v>
+      </c>
+      <c r="S1">
+        <v>2032</v>
+      </c>
+      <c r="T1">
+        <v>2033</v>
+      </c>
+      <c r="U1">
+        <v>2034</v>
+      </c>
+      <c r="V1">
+        <v>2035</v>
+      </c>
+      <c r="W1">
+        <v>2036</v>
+      </c>
+      <c r="X1">
+        <v>2037</v>
+      </c>
+      <c r="Y1">
+        <v>2038</v>
+      </c>
+      <c r="Z1">
+        <v>2039</v>
+      </c>
+      <c r="AA1">
+        <v>2040</v>
+      </c>
+      <c r="AB1">
+        <v>2041</v>
+      </c>
+      <c r="AC1">
+        <v>2042</v>
+      </c>
+      <c r="AD1">
+        <v>2043</v>
+      </c>
+      <c r="AE1">
+        <v>2044</v>
+      </c>
+      <c r="AF1">
+        <v>2045</v>
+      </c>
+      <c r="AG1">
+        <v>2046</v>
+      </c>
+      <c r="AH1">
+        <v>2047</v>
+      </c>
+      <c r="AI1">
+        <v>2048</v>
+      </c>
+      <c r="AJ1">
+        <v>2049</v>
+      </c>
+      <c r="AK1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1.67</v>
+      </c>
+      <c r="C2">
+        <v>1.67</v>
+      </c>
+      <c r="D2">
+        <v>1.67</v>
+      </c>
+      <c r="E2">
+        <v>1.67</v>
+      </c>
+      <c r="F2">
+        <v>1.67</v>
+      </c>
+      <c r="G2">
+        <v>1.67</v>
+      </c>
+      <c r="H2">
+        <v>1.67</v>
+      </c>
+      <c r="I2">
+        <v>1.67</v>
+      </c>
+      <c r="J2">
+        <v>1.67</v>
+      </c>
+      <c r="K2">
+        <v>1.67</v>
+      </c>
+      <c r="L2">
+        <v>1.67</v>
+      </c>
+      <c r="M2">
+        <v>1.67</v>
+      </c>
+      <c r="N2">
+        <v>1.67</v>
+      </c>
+      <c r="O2">
+        <v>1.67</v>
+      </c>
+      <c r="P2">
+        <v>1.67</v>
+      </c>
+      <c r="Q2">
+        <v>1.67</v>
+      </c>
+      <c r="R2">
+        <v>1.67</v>
+      </c>
+      <c r="S2">
+        <v>1.67</v>
+      </c>
+      <c r="T2">
+        <v>1.67</v>
+      </c>
+      <c r="U2">
+        <v>1.67</v>
+      </c>
+      <c r="V2">
+        <v>1.67</v>
+      </c>
+      <c r="W2">
+        <v>1.67</v>
+      </c>
+      <c r="X2">
+        <v>1.67</v>
+      </c>
+      <c r="Y2">
+        <v>1.67</v>
+      </c>
+      <c r="Z2">
+        <v>1.67</v>
+      </c>
+      <c r="AA2">
+        <v>1.67</v>
+      </c>
+      <c r="AB2">
+        <v>1.67</v>
+      </c>
+      <c r="AC2">
+        <v>1.67</v>
+      </c>
+      <c r="AD2">
+        <v>1.67</v>
+      </c>
+      <c r="AE2">
+        <v>1.67</v>
+      </c>
+      <c r="AF2">
+        <v>1.67</v>
+      </c>
+      <c r="AG2">
+        <v>1.67</v>
+      </c>
+      <c r="AH2">
+        <v>1.67</v>
+      </c>
+      <c r="AI2">
+        <v>1.67</v>
+      </c>
+      <c r="AJ2">
+        <v>1.67</v>
+      </c>
+      <c r="AK2">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="C3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="D3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="E3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="F3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="G3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="H3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="I3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="J3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="K3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="L3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="M3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="N3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="O3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="P3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="Q3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="R3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="S3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="T3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="U3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="V3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="W3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="X3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="Y3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="Z3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AA3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AB3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AC3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AD3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AE3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AF3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AG3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AH3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AI3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AJ3">
+        <v>21.196137258578663</v>
+      </c>
+      <c r="AK3">
+        <v>21.196137258578663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="C4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="D4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="E4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="F4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="G4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="H4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="I4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="J4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="K4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="L4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="M4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="N4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="O4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="P4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="Q4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="R4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="S4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="T4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="U4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="V4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="W4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="X4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="Y4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="Z4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AA4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AB4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AC4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AD4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AE4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AF4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AG4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AH4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AI4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AJ4">
+        <v>111.39416306433705</v>
+      </c>
+      <c r="AK4">
+        <v>111.39416306433705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="C5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="D5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="E5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="F5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="G5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="H5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="I5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="J5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="K5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="L5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="M5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="N5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="O5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="P5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Q5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="R5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="S5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="T5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="U5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="V5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="W5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="X5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Y5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Z5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AA5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AB5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AC5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AD5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AE5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AF5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AG5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AH5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AI5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AJ5">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AK5">
+        <v>486.56731685074101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="C7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="D7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="E7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="F7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="G7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="H7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="I7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="J7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="K7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="L7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="M7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="N7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="O7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="P7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="Q7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="R7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="S7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="T7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="U7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="V7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="W7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="X7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="Y7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="Z7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AA7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AB7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AC7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AD7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AE7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AF7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AG7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AH7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AI7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AJ7">
+        <v>1.2700756740871355</v>
+      </c>
+      <c r="AK7">
+        <v>1.2700756740871355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>2016</v>
+      </c>
+      <c r="C9">
+        <v>2017</v>
+      </c>
+      <c r="D9">
+        <v>2018</v>
+      </c>
+      <c r="E9">
+        <v>2019</v>
+      </c>
+      <c r="F9">
+        <v>2020</v>
+      </c>
+      <c r="G9">
+        <v>2021</v>
+      </c>
+      <c r="H9">
+        <v>2022</v>
+      </c>
+      <c r="I9">
+        <v>2023</v>
+      </c>
+      <c r="J9">
+        <v>2024</v>
+      </c>
+      <c r="K9">
+        <v>2025</v>
+      </c>
+      <c r="L9">
+        <v>2026</v>
+      </c>
+      <c r="M9">
+        <v>2027</v>
+      </c>
+      <c r="N9">
+        <v>2028</v>
+      </c>
+      <c r="O9">
+        <v>2029</v>
+      </c>
+      <c r="P9">
+        <v>2030</v>
+      </c>
+      <c r="Q9">
+        <v>2031</v>
+      </c>
+      <c r="R9">
+        <v>2032</v>
+      </c>
+      <c r="S9">
+        <v>2033</v>
+      </c>
+      <c r="T9">
+        <v>2034</v>
+      </c>
+      <c r="U9">
+        <v>2035</v>
+      </c>
+      <c r="V9">
+        <v>2036</v>
+      </c>
+      <c r="W9">
+        <v>2037</v>
+      </c>
+      <c r="X9">
+        <v>2038</v>
+      </c>
+      <c r="Y9">
+        <v>2039</v>
+      </c>
+      <c r="Z9">
+        <v>2040</v>
+      </c>
+      <c r="AA9">
+        <v>2041</v>
+      </c>
+      <c r="AB9">
+        <v>2042</v>
+      </c>
+      <c r="AC9">
+        <v>2043</v>
+      </c>
+      <c r="AD9">
+        <v>2044</v>
+      </c>
+      <c r="AE9">
+        <v>2045</v>
+      </c>
+      <c r="AF9">
+        <v>2046</v>
+      </c>
+      <c r="AG9">
+        <v>2047</v>
+      </c>
+      <c r="AH9">
+        <v>2048</v>
+      </c>
+      <c r="AI9">
+        <v>2049</v>
+      </c>
+      <c r="AJ9">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <v>1</v>
+      </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>16</v>
+      </c>
+      <c r="M11">
+        <v>16</v>
+      </c>
+      <c r="N11">
+        <v>16</v>
+      </c>
+      <c r="O11">
+        <v>16</v>
+      </c>
+      <c r="P11">
+        <v>16</v>
+      </c>
+      <c r="Q11">
+        <v>16</v>
+      </c>
+      <c r="R11">
+        <v>16</v>
+      </c>
+      <c r="S11">
+        <v>16</v>
+      </c>
+      <c r="T11">
+        <v>16</v>
+      </c>
+      <c r="U11">
+        <v>16</v>
+      </c>
+      <c r="V11">
+        <v>16</v>
+      </c>
+      <c r="W11">
+        <v>16</v>
+      </c>
+      <c r="X11">
+        <v>16</v>
+      </c>
+      <c r="Y11">
+        <v>16</v>
+      </c>
+      <c r="Z11">
+        <v>16</v>
+      </c>
+      <c r="AA11">
+        <v>16</v>
+      </c>
+      <c r="AB11">
+        <v>16</v>
+      </c>
+      <c r="AC11">
+        <v>16</v>
+      </c>
+      <c r="AD11">
+        <v>16</v>
+      </c>
+      <c r="AE11">
+        <v>16</v>
+      </c>
+      <c r="AF11">
+        <v>16</v>
+      </c>
+      <c r="AG11">
+        <v>16</v>
+      </c>
+      <c r="AH11">
+        <v>16</v>
+      </c>
+      <c r="AI11">
+        <v>16</v>
+      </c>
+      <c r="AJ11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="C12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="D12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="E12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="F12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="G12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="H12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="I12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="J12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="K12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="L12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="M12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="N12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="O12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="P12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="Q12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="R12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="S12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="T12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="U12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="V12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="W12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="X12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="Y12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="Z12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AA12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AB12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AC12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AD12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AE12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AF12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AG12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AH12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AI12">
+        <v>41.989116133258747</v>
+      </c>
+      <c r="AJ12">
+        <v>41.989116133258747</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="C13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="D13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="E13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="F13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="G13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="H13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="I13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="J13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="K13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="L13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="M13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="N13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="O13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="P13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="Q13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="R13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="S13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="T13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="U13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="V13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="W13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="X13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="Y13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="Z13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AA13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AB13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AC13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AD13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AE13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AF13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AG13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AH13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AI13">
+        <v>3512.35916421195</v>
+      </c>
+      <c r="AJ13">
+        <v>3512.35916421195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="C14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="D14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="E14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="F14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="G14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="H14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="I14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="J14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="K14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="L14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="M14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="N14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="O14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="P14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="Q14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="R14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="S14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="T14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="U14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="V14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="W14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="X14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="Y14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="Z14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AA14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AB14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AC14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AD14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AE14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AF14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AG14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AH14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AI14">
+        <v>1974.4736422180429</v>
+      </c>
+      <c r="AJ14">
+        <v>1974.4736422180429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -6087,7 +7665,7 @@
   <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7072,15 +8650,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7782,109 +9360,144 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="S6" s="3">
+      <c r="S6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="U6" s="3">
+      <c r="U6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="V6" s="3">
+      <c r="V6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="W6" s="3">
+      <c r="W6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="X6" s="3">
+      <c r="X6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="Z6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AA6" s="3">
+      <c r="AA6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AB6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AC6" s="3">
+      <c r="AC6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AD6" s="3">
+      <c r="AD6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AE6" s="3">
+      <c r="AE6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AF6" s="3">
+      <c r="AF6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AG6" s="3">
+      <c r="AG6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AH6" s="3">
+      <c r="AH6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="AI6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
-      <c r="AJ6" s="3">
+      <c r="AJ6" s="147">
+        <f>'US AVLo'!$B$14</f>
         <v>1974.4736422180429</v>
       </c>
     </row>

</xml_diff>